<commit_message>
Sheet names are case-insensitive
</commit_message>
<xml_diff>
--- a/src/test/resources/named_sheets.xlsx
+++ b/src/test/resources/named_sheets.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Czarek\Documents\Projects\poiji\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3725A453-0B8D-4C99-B1A7-5E234622A36E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9925BEB-E362-4A7B-81D3-13819074EE85}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="0" windowWidth="19500" windowHeight="8115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet #1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet #2" sheetId="1" r:id="rId2"/>
+    <sheet name="sHEeT #1" sheetId="2" r:id="rId1"/>
+    <sheet name="sHEeT #2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>

</xml_diff>